<commit_message>
Un-do 1.025;Assume "no titles" if autodetect fails
</commit_message>
<xml_diff>
--- a/tlib/Multisheet.xlsx
+++ b/tlib/Multisheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="PresidentsSheet" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="OtherSheetA" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="AddrListSheet" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="PresidentsSheet" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="EmptySheet" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="AddrListSheet" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -448,24 +448,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -481,8 +485,114 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -494,19 +604,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="20.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="55.22"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -514,10 +624,10 @@
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -525,10 +635,10 @@
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -536,10 +646,10 @@
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -547,10 +657,10 @@
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -558,10 +668,10 @@
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -569,10 +679,10 @@
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -580,10 +690,10 @@
       <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -591,10 +701,10 @@
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -602,10 +712,10 @@
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -613,10 +723,10 @@
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -624,10 +734,10 @@
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -635,10 +745,10 @@
       <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -646,10 +756,10 @@
       <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -657,10 +767,10 @@
       <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -668,10 +778,10 @@
       <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -679,10 +789,10 @@
       <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -690,10 +800,10 @@
       <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -701,10 +811,10 @@
       <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="2" t="s">
         <v>37</v>
       </c>
     </row>
@@ -712,10 +822,10 @@
       <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -723,10 +833,10 @@
       <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="2" t="s">
         <v>41</v>
       </c>
     </row>
@@ -734,10 +844,10 @@
       <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="2" t="s">
         <v>43</v>
       </c>
     </row>
@@ -745,10 +855,10 @@
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="2" t="s">
         <v>46</v>
       </c>
     </row>
@@ -756,10 +866,10 @@
       <c r="A24" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="2" t="s">
         <v>48</v>
       </c>
     </row>
@@ -767,10 +877,10 @@
       <c r="A25" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -778,10 +888,10 @@
       <c r="A26" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="2" t="s">
         <v>52</v>
       </c>
     </row>
@@ -789,10 +899,10 @@
       <c r="A27" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="2" t="s">
         <v>54</v>
       </c>
     </row>
@@ -800,10 +910,10 @@
       <c r="A28" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="2" t="s">
         <v>56</v>
       </c>
     </row>
@@ -811,10 +921,10 @@
       <c r="A29" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="2" t="s">
         <v>58</v>
       </c>
     </row>
@@ -822,10 +932,10 @@
       <c r="A30" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="2" t="s">
         <v>60</v>
       </c>
     </row>
@@ -833,10 +943,10 @@
       <c r="A31" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="2" t="s">
         <v>62</v>
       </c>
     </row>
@@ -844,10 +954,10 @@
       <c r="A32" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="2" t="s">
         <v>64</v>
       </c>
     </row>
@@ -855,10 +965,10 @@
       <c r="A33" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="2" t="s">
         <v>66</v>
       </c>
     </row>
@@ -866,10 +976,10 @@
       <c r="A34" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" s="2" t="s">
         <v>68</v>
       </c>
     </row>
@@ -877,10 +987,10 @@
       <c r="A35" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" s="2" t="s">
         <v>70</v>
       </c>
     </row>
@@ -888,10 +998,10 @@
       <c r="A36" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="2" t="s">
         <v>72</v>
       </c>
     </row>
@@ -899,10 +1009,10 @@
       <c r="A37" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -910,10 +1020,10 @@
       <c r="A38" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" s="2" t="s">
         <v>76</v>
       </c>
     </row>
@@ -921,10 +1031,10 @@
       <c r="A39" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="2" t="s">
         <v>78</v>
       </c>
     </row>
@@ -932,10 +1042,10 @@
       <c r="A40" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" s="2" t="s">
         <v>80</v>
       </c>
     </row>
@@ -943,10 +1053,10 @@
       <c r="A41" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" s="2" t="s">
         <v>82</v>
       </c>
     </row>
@@ -954,10 +1064,10 @@
       <c r="A42" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="C42" s="2" t="s">
         <v>84</v>
       </c>
     </row>
@@ -965,10 +1075,10 @@
       <c r="A43" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" s="2" t="s">
         <v>86</v>
       </c>
     </row>
@@ -976,10 +1086,10 @@
       <c r="A44" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" s="2" t="s">
         <v>88</v>
       </c>
     </row>
@@ -987,10 +1097,10 @@
       <c r="A45" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" s="2" t="s">
         <v>90</v>
       </c>
     </row>
@@ -998,10 +1108,10 @@
       <c r="A46" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="2" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1017,13 +1127,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1040,110 +1150,110 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="12.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="19.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="19.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="11.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="6.45"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="2" t="n">
         <v>12946</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="2" t="n">
         <v>19133</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="2" t="n">
         <v>13021</v>
       </c>
     </row>

</xml_diff>